<commit_message>
haciendo las pruebas finales y agregando color a la consola para distinguir un poco los mensajes
</commit_message>
<xml_diff>
--- a/game_stats.xlsx
+++ b/game_stats.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,13 +413,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -441,6 +442,7 @@
         </is>
       </c>
     </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
@@ -471,216 +473,32 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ALberto</t>
+          <t>Alberto</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>15</v>
-      </c>
-      <c r="D6" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Iliana</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>25</v>
-      </c>
-      <c r="C7" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Ayme</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>25</v>
-      </c>
-      <c r="C8" t="n">
-        <v>15</v>
-      </c>
-      <c r="D8" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Mary</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>25</v>
-      </c>
-      <c r="C9" t="n">
-        <v>15</v>
-      </c>
-      <c r="D9" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Luis</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>25</v>
-      </c>
-      <c r="C10" t="n">
-        <v>15</v>
-      </c>
-      <c r="D10" t="n">
-        <v>10</v>
-      </c>
-      <c r="E10" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Pedro</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>25</v>
-      </c>
-      <c r="C11" t="n">
-        <v>15</v>
-      </c>
-      <c r="D11" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Carmen</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>25</v>
-      </c>
-      <c r="C12" t="n">
-        <v>15</v>
-      </c>
-      <c r="D12" t="n">
-        <v>10</v>
-      </c>
-      <c r="E12" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Julian</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>25</v>
-      </c>
-      <c r="C13" t="n">
-        <v>15</v>
-      </c>
-      <c r="D13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E13" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Pepe</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>27</v>
-      </c>
-      <c r="C14" t="n">
-        <v>16</v>
-      </c>
-      <c r="D14" t="n">
-        <v>11</v>
-      </c>
-      <c r="E14" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Melon</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Melames</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>The king</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
haciendo los ajustes finales al juego
</commit_message>
<xml_diff>
--- a/game_stats.xlsx
+++ b/game_stats.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -442,7 +441,6 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
@@ -500,6 +498,38 @@
       </c>
       <c r="E7" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ruben</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Jacob</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>